<commit_message>
Renamed the variables in the health insurance spreadsheet
</commit_message>
<xml_diff>
--- a/health_insurance.xlsx
+++ b/health_insurance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ezulu Priscilla\Desktop\EHIC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/muhammad/Documents/DevProjects/DSN/health-worker-allocation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B33347E-31A3-480B-8E06-BFA1BB716139}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39D07E6-DFCE-0148-BB77-58A12C168ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,15 +38,6 @@
     <t>LGA</t>
   </si>
   <si>
-    <t>In-patient</t>
-  </si>
-  <si>
-    <t>enrollment_rate</t>
-  </si>
-  <si>
-    <t>death_rate</t>
-  </si>
-  <si>
     <t>Akoko-Edo</t>
   </si>
   <si>
@@ -104,7 +95,16 @@
     <t>Population</t>
   </si>
   <si>
-    <t>OutPatient</t>
+    <t>Outpatient</t>
+  </si>
+  <si>
+    <t>Enrollment Rate</t>
+  </si>
+  <si>
+    <t>Death Rate</t>
+  </si>
+  <si>
+    <t>Inpatient</t>
   </si>
 </sst>
 </file>
@@ -114,7 +114,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +131,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -169,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -178,6 +184,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,42 +492,42 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.21875" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" customWidth="1"/>
-    <col min="5" max="5" width="14.21875" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
       </c>
       <c r="B2" s="2">
         <v>386400</v>
@@ -536,9 +545,9 @@
         <v>0.13457556935817805</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>502700</v>
@@ -556,9 +565,9 @@
         <v>0.80962800875273522</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
         <v>155500</v>
@@ -576,9 +585,9 @@
         <v>4.5337620578778139</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
         <v>180200</v>
@@ -596,9 +605,9 @@
         <v>8.3240843507214196E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
         <v>245700</v>
@@ -616,9 +625,9 @@
         <v>8.5470085470085472E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7" s="2">
         <v>188700</v>
@@ -636,9 +645,9 @@
         <v>2.1197668256491786E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2">
         <v>139200</v>
@@ -656,9 +665,9 @@
         <v>7.9022988505747127E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2">
         <v>217700</v>
@@ -676,9 +685,9 @@
         <v>0.1148369315571888</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2">
         <v>294000</v>
@@ -696,9 +705,9 @@
         <v>5.1020408163265307E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2">
         <v>103800</v>
@@ -716,9 +725,9 @@
         <v>0.11560693641618497</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2">
         <v>549700</v>
@@ -736,9 +745,9 @@
         <v>2.1830089139530651E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2">
         <v>553300</v>
@@ -756,9 +765,9 @@
         <v>0.26748599313211641</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2">
         <v>271800</v>
@@ -776,9 +785,9 @@
         <v>8.4621044885945546E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2">
         <v>229500</v>
@@ -796,9 +805,9 @@
         <v>6.1002178649237473E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2">
         <v>204000</v>
@@ -816,9 +825,9 @@
         <v>0.18627450980392157</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2">
         <v>228500</v>
@@ -836,9 +845,9 @@
         <v>0.2932166301969365</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2">
         <v>146300</v>
@@ -856,9 +865,9 @@
         <v>4.784688995215311E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2">
         <v>180000</v>

</xml_diff>